<commit_message>
more tests for calibration
</commit_message>
<xml_diff>
--- a/Test/05-26-17_B7A_yeast_td_fract5_rep1.xlsx
+++ b/Test/05-26-17_B7A_yeast_td_fract5_rep1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -508,7 +508,7 @@
   <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -587,7 +587,7 @@
         <v>44.580977000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -601,7 +601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>6</v>
       </c>
@@ -615,7 +615,7 @@
         <v>6999.0086000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>7</v>
       </c>
@@ -629,7 +629,7 @@
         <v>6999.0082000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>8</v>
       </c>
@@ -643,7 +643,7 @@
         <v>6999.0092000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>9</v>
       </c>
@@ -657,7 +657,7 @@
         <v>6999.0099</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>10</v>
       </c>
@@ -671,7 +671,7 @@
         <v>6999.0092999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>11</v>
       </c>
@@ -685,7 +685,7 @@
         <v>6999.0084999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>12</v>
       </c>
@@ -699,7 +699,7 @@
         <v>6999.0096000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>13</v>
       </c>
@@ -713,7 +713,7 @@
         <v>6999.0110000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>14</v>
       </c>
@@ -727,7 +727,7 @@
         <v>6999.0097999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -762,7 +762,7 @@
         <v>44.373942</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="19.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -776,7 +776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>6</v>
       </c>
@@ -790,7 +790,7 @@
         <v>6999.0060000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>7</v>
       </c>
@@ -804,7 +804,7 @@
         <v>6999.0065999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>8</v>
       </c>
@@ -818,7 +818,7 @@
         <v>6999.0088999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>9</v>
       </c>
@@ -832,7 +832,7 @@
         <v>6999.0087999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>10</v>
       </c>
@@ -846,7 +846,7 @@
         <v>6999.0084999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>11</v>
       </c>
@@ -860,7 +860,7 @@
         <v>6999.009</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>12</v>
       </c>
@@ -874,7 +874,7 @@
         <v>6999.0097999999989</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>13</v>
       </c>
@@ -888,7 +888,7 @@
         <v>6999.0113000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>14</v>
       </c>
@@ -902,7 +902,7 @@
         <v>6999.0101000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -937,7 +937,7 @@
         <v>44.742062500000003</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="19.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="19.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -951,7 +951,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>6</v>
       </c>
@@ -965,7 +965,7 @@
         <v>6999.0081</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>7</v>
       </c>
@@ -979,7 +979,7 @@
         <v>6999.0079999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>8</v>
       </c>
@@ -993,7 +993,7 @@
         <v>6999.0092000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>9</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>6999.0093999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>10</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>6999.0081</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>11</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>6999.0081</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>12</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>6999.0091999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>13</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>6999.0108</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>14</v>
       </c>
@@ -1077,12 +1077,12 @@
         <v>6999.0101999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
-      <c r="B35" s="3">
-        <v>6533.6971999999996</v>
+      <c r="B35">
+        <v>6533.6713346899996</v>
       </c>
       <c r="C35" s="1">
         <v>18619903.52</v>
@@ -1112,7 +1112,7 @@
         <v>44.151167999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="19.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="19.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>24</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>6</v>
       </c>
@@ -1134,13 +1134,14 @@
         <v>557549.78</v>
       </c>
       <c r="D37" s="3">
-        <v>1089.95552</v>
-      </c>
-      <c r="E37" s="3">
-        <v>6533.6772000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f>(E37+B37*1.007276474)/B37</f>
+        <v>1089.9524989223332</v>
+      </c>
+      <c r="E37">
+        <v>6533.6713346899996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>7</v>
       </c>
@@ -1148,13 +1149,14 @@
         <v>2242570.1800000002</v>
       </c>
       <c r="D38" s="3">
-        <v>934.39148999999998</v>
-      </c>
-      <c r="E38" s="3">
-        <v>6533.6773999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D38:D44" si="0">(E38+B38*1.007276474)/B38</f>
+        <v>934.38889571542848</v>
+      </c>
+      <c r="E38">
+        <v>6533.6713346899996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>8</v>
       </c>
@@ -1162,13 +1164,14 @@
         <v>3510374.16</v>
       </c>
       <c r="D39" s="3">
-        <v>817.71846000000005</v>
-      </c>
-      <c r="E39" s="3">
-        <v>6533.6787000000004</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>817.71619331024999</v>
+      </c>
+      <c r="E39">
+        <v>6533.6713346899996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>9</v>
       </c>
@@ -1176,13 +1179,14 @@
         <v>7316271.3399999999</v>
       </c>
       <c r="D40" s="3">
-        <v>726.97276999999997</v>
-      </c>
-      <c r="E40" s="3">
-        <v>6533.6773000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>726.97075810622221</v>
+      </c>
+      <c r="E40">
+        <v>6533.6713346899996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>10</v>
       </c>
@@ -1190,13 +1194,14 @@
         <v>21604149.390000001</v>
       </c>
       <c r="D41" s="3">
-        <v>654.37621999999999</v>
-      </c>
-      <c r="E41" s="3">
-        <v>6533.6783000000005</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>654.37440994299993</v>
+      </c>
+      <c r="E41">
+        <v>6533.6713346899996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>11</v>
       </c>
@@ -1204,13 +1209,14 @@
         <v>60692639.909999996</v>
       </c>
       <c r="D42" s="3">
-        <v>594.97905000000003</v>
-      </c>
-      <c r="E42" s="3">
-        <v>6533.6787000000004</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>594.97739780945449</v>
+      </c>
+      <c r="E42">
+        <v>6533.6713346899996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>12</v>
       </c>
@@ -1218,13 +1224,14 @@
         <v>70344813.980000004</v>
       </c>
       <c r="D43" s="3">
-        <v>545.48140000000001</v>
-      </c>
-      <c r="E43" s="3">
-        <v>6533.6756999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>545.47988769816664</v>
+      </c>
+      <c r="E43">
+        <v>6533.6713346899996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>13</v>
       </c>
@@ -1232,10 +1239,11 @@
         <v>44393701.149999999</v>
       </c>
       <c r="D44" s="3">
-        <v>503.59877</v>
-      </c>
-      <c r="E44" s="3">
-        <v>6533.6755000000003</v>
+        <f t="shared" si="0"/>
+        <v>503.59737914246153</v>
+      </c>
+      <c r="E44">
+        <v>6533.6713346899996</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">

</xml_diff>